<commit_message>
Update shepherd_v2.4 - bestand.xlsx
</commit_message>
<xml_diff>
--- a/PCBs_old/shepherd_cape_v2.4b/shepherd_v2.4 - bestand.xlsx
+++ b/PCBs_old/shepherd_cape_v2.4b/shepherd_v2.4 - bestand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmo\Documents\GitHub\shepherd_v2_planning\PCBs\shepherd_cape_v2.4b\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmo\Documents\GitHub\shepherd_v2_planning\PCBs_old\shepherd_cape_v2.4b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5585197-05D5-4D5A-9848-B00C5999A0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C69D39-8A3C-4C84-803A-DD72ADC545C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1092" yWindow="132" windowWidth="23316" windowHeight="23676" xr2:uid="{1B8282AA-D0AE-43C3-9486-CC1A757A3883}"/>
+    <workbookView xWindow="315" yWindow="3780" windowWidth="19725" windowHeight="28335" xr2:uid="{1B8282AA-D0AE-43C3-9486-CC1A757A3883}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-shepherd_v2" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="384">
   <si>
     <t>Comment</t>
   </si>
@@ -1176,6 +1168,18 @@
   </si>
   <si>
     <t>UD_PI5A4158ZA</t>
+  </si>
+  <si>
+    <t>2023-09</t>
+  </si>
+  <si>
+    <t>,+100More</t>
+  </si>
+  <si>
+    <t>,+200More</t>
+  </si>
+  <si>
+    <t>240R,+1000More</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -1267,6 +1271,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1584,26 +1589,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+      <selection activeCell="P51" sqref="P51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1649,8 +1654,11 @@
       <c r="O1" s="4" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1696,7 +1704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>361</v>
       </c>
@@ -1776,7 +1784,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1819,7 +1827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1861,7 +1869,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>37</v>
       </c>
@@ -1901,7 +1909,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -1941,7 +1949,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1987,7 +1995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -2027,7 +2035,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>61</v>
       </c>
@@ -2067,7 +2075,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
     </row>
-    <row r="12" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>66</v>
       </c>
@@ -2107,7 +2115,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>72</v>
       </c>
@@ -2149,7 +2157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>79</v>
       </c>
@@ -2186,7 +2194,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>86</v>
       </c>
@@ -2223,7 +2231,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>92</v>
       </c>
@@ -2263,7 +2271,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>99</v>
       </c>
@@ -2303,7 +2311,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -2340,7 +2348,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>112</v>
       </c>
@@ -2377,7 +2385,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>118</v>
       </c>
@@ -2417,7 +2425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>123</v>
       </c>
@@ -2457,7 +2465,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>129</v>
       </c>
@@ -2497,7 +2505,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>134</v>
       </c>
@@ -2537,7 +2545,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>137</v>
       </c>
@@ -2577,7 +2585,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>143</v>
       </c>
@@ -2617,7 +2625,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>151</v>
       </c>
@@ -2654,7 +2662,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>158</v>
       </c>
@@ -2694,7 +2702,7 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
     </row>
-    <row r="28" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>165</v>
       </c>
@@ -2734,7 +2742,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
     </row>
-    <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>171</v>
       </c>
@@ -2774,7 +2782,7 @@
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
     </row>
-    <row r="30" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>173</v>
       </c>
@@ -2814,7 +2822,7 @@
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>180</v>
       </c>
@@ -2851,7 +2859,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>187</v>
       </c>
@@ -2891,7 +2899,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>192</v>
       </c>
@@ -2934,7 +2942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>197</v>
       </c>
@@ -2971,7 +2979,7 @@
       </c>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>204</v>
       </c>
@@ -3014,7 +3022,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>209</v>
       </c>
@@ -3052,8 +3060,11 @@
       <c r="L36" s="10" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P36" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>214</v>
       </c>
@@ -3095,7 +3106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>219</v>
       </c>
@@ -3134,7 +3145,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>224</v>
       </c>
@@ -3170,8 +3181,11 @@
       <c r="L39" s="10" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P39" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>227</v>
       </c>
@@ -3213,7 +3227,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>232</v>
       </c>
@@ -3257,8 +3271,11 @@
       <c r="N41">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P41" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>237</v>
       </c>
@@ -3295,7 +3312,7 @@
       </c>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>242</v>
       </c>
@@ -3332,7 +3349,7 @@
       </c>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>247</v>
       </c>
@@ -3372,7 +3389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>366</v>
       </c>
@@ -3409,7 +3426,7 @@
       </c>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>257</v>
       </c>
@@ -3446,7 +3463,7 @@
       </c>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>263</v>
       </c>
@@ -3486,7 +3503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>367</v>
       </c>
@@ -3526,7 +3543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>274</v>
       </c>
@@ -3564,8 +3581,11 @@
       <c r="L49" s="10" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49" s="11">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>279</v>
       </c>
@@ -3603,8 +3623,11 @@
       <c r="L50" s="10" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50" s="11">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>369</v>
       </c>
@@ -3650,7 +3673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>370</v>
       </c>
@@ -3686,8 +3709,11 @@
       <c r="L52" s="10" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P52" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>375</v>
       </c>
@@ -3727,7 +3753,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>296</v>
       </c>
@@ -3767,7 +3793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>302</v>
       </c>
@@ -3810,7 +3836,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>376</v>
       </c>
@@ -3853,7 +3879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>377</v>
       </c>
@@ -3893,7 +3919,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>316</v>
       </c>
@@ -3933,7 +3959,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>321</v>
       </c>
@@ -3973,7 +3999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>325</v>
       </c>
@@ -4013,7 +4039,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>330</v>
       </c>
@@ -4053,7 +4079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>334</v>
       </c>
@@ -4096,7 +4122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>378</v>
       </c>
@@ -4133,7 +4159,7 @@
       </c>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>379</v>
       </c>

</xml_diff>